<commit_message>
added the user`s transition to their page
</commit_message>
<xml_diff>
--- a/client/public/Sorce/balanceDP.xlsx
+++ b/client/public/Sorce/balanceDP.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/SharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="414">
   <si>
     <t>Формирвоание отчета</t>
   </si>
   <si>
-    <t>Период: на 31.01.2025 12:25:13</t>
+    <t>Период: на 01.02.2025 11:35:11</t>
   </si>
   <si>
     <t>Показатели: Свободный остаток(В ед. хранения);</t>
@@ -371,12 +371,18 @@
     <t>Wafers горіх ВКФ 72г /22шт AR /</t>
   </si>
   <si>
+    <t>Wafers горіх ВКФ 72г /22шт AR /АКЦІЯ ВІП 1</t>
+  </si>
+  <si>
     <t>Wafers горіх ККФ 216г /16шт</t>
   </si>
   <si>
     <t>Wafers какао ВКФ 72г /22шт AR /</t>
   </si>
   <si>
+    <t>Wafers какао ВКФ 72г /22шт AR /АКЦІЯ ВІП 1</t>
+  </si>
+  <si>
     <t>Wafers какао ККФ 216г /16шт</t>
   </si>
   <si>
@@ -404,6 +410,9 @@
     <t>Wafers молоко ВКФ 72г /22шт AR /АКЦІЯ</t>
   </si>
   <si>
+    <t>Wafers молоко ВКФ 72г /22шт AR /АКЦІЯ ВІП 1</t>
+  </si>
+  <si>
     <t>Wafers молоко ККФ 216г /16шт</t>
   </si>
   <si>
@@ -1182,9 +1191,6 @@
   </si>
   <si>
     <t>Roshen Nut чорний з цілим мигдалем ВКФ 90г /20шт</t>
-  </si>
-  <si>
-    <t>Roshen Nut чорний з цілим мигдалем ВКФ 90г /20шт АКЦІЯ Цінова</t>
   </si>
   <si>
     <t>Roshen Nut чорний з цілим мигдалем ВКФ 90г /20шт АКЦІЯ Цінова UA</t>
@@ -1496,7 +1502,7 @@
     <outlinePr summaryBelow="false" summaryRight="false"/>
     <pageSetUpPr autoPageBreaks="false"/>
   </sheetPr>
-  <dimension ref="C412"/>
+  <dimension ref="C414"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
@@ -1572,7 +1578,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>570195</v>
+        <v>540421</v>
       </c>
     </row>
     <row r="13" ht="11" customHeight="true" outlineLevel="1">
@@ -1580,7 +1586,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>100053</v>
+        <v>93475</v>
       </c>
     </row>
     <row r="14" ht="11" customHeight="true" outlineLevel="2">
@@ -1588,7 +1594,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>17142</v>
+        <v>15686</v>
       </c>
     </row>
     <row r="15" ht="11" customHeight="true" outlineLevel="3">
@@ -1596,7 +1602,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="16" t="n">
-        <v>2396</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="16" ht="11" customHeight="true" outlineLevel="3">
@@ -1604,7 +1610,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="11" t="n">
-        <v>730</v>
+        <v>644</v>
       </c>
     </row>
     <row r="17" ht="11" customHeight="true" outlineLevel="3">
@@ -1612,7 +1618,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="16" t="n">
-        <v>1504</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="18" ht="11" customHeight="true" outlineLevel="3">
@@ -1620,7 +1626,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="16" t="n">
-        <v>2794</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="19" ht="11" customHeight="true" outlineLevel="3">
@@ -1628,7 +1634,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="16" t="n">
-        <v>1259</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="20" ht="11" customHeight="true" outlineLevel="3">
@@ -1636,7 +1642,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="11" t="n">
-        <v>730</v>
+        <v>644</v>
       </c>
     </row>
     <row r="21" ht="11" customHeight="true" outlineLevel="3">
@@ -1644,7 +1650,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="16" t="n">
-        <v>1921</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="22" ht="11" customHeight="true" outlineLevel="3">
@@ -1652,7 +1658,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="11" t="n">
-        <v>710</v>
+        <v>634</v>
       </c>
     </row>
     <row r="23" ht="11" customHeight="true" outlineLevel="3">
@@ -1660,7 +1666,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="16" t="n">
-        <v>2058</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="24" ht="11" customHeight="true" outlineLevel="3">
@@ -1668,7 +1674,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="16" t="n">
-        <v>3040</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="25" ht="11" customHeight="true" outlineLevel="2">
@@ -1676,7 +1682,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="12" t="n">
-        <v>26686</v>
+        <v>24497</v>
       </c>
     </row>
     <row r="26" ht="11" customHeight="true" outlineLevel="3">
@@ -1684,7 +1690,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="16" t="n">
-        <v>1835</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="27" ht="11" customHeight="true" outlineLevel="3">
@@ -1692,7 +1698,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="16" t="n">
-        <v>22997</v>
+        <v>21912</v>
       </c>
     </row>
     <row r="28" ht="11" customHeight="true" outlineLevel="3">
@@ -1708,7 +1714,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="16" t="n">
-        <v>1297</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="30" ht="11" customHeight="true" outlineLevel="3">
@@ -1716,7 +1722,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="11" t="n">
-        <v>548</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" ht="11" customHeight="true" outlineLevel="2">
@@ -1724,7 +1730,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="12" t="n">
-        <v>16190</v>
+        <v>15351</v>
       </c>
     </row>
     <row r="32" ht="11" customHeight="true" outlineLevel="3">
@@ -1732,7 +1738,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="11" t="n">
-        <v>879</v>
+        <v>858</v>
       </c>
     </row>
     <row r="33" ht="11" customHeight="true" outlineLevel="3">
@@ -1748,7 +1754,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="16" t="n">
-        <v>1229</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="35" ht="11" customHeight="true" outlineLevel="3">
@@ -1764,7 +1770,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="11" t="n">
-        <v>940</v>
+        <v>863</v>
       </c>
     </row>
     <row r="37" ht="11" customHeight="true" outlineLevel="3">
@@ -1780,7 +1786,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="11" t="n">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" ht="11" customHeight="true" outlineLevel="3">
@@ -1788,7 +1794,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="11" t="n">
-        <v>547</v>
+        <v>515</v>
       </c>
     </row>
     <row r="40" ht="11" customHeight="true" outlineLevel="3">
@@ -1796,7 +1802,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="11" t="n">
-        <v>885</v>
+        <v>860</v>
       </c>
     </row>
     <row r="41" ht="11" customHeight="true" outlineLevel="3">
@@ -1812,7 +1818,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="16" t="n">
-        <v>2298</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="43" ht="11" customHeight="true" outlineLevel="3">
@@ -1828,7 +1834,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="16" t="n">
-        <v>1023</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="45" ht="11" customHeight="true" outlineLevel="3">
@@ -1844,7 +1850,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="11" t="n">
-        <v>720</v>
+        <v>710</v>
       </c>
     </row>
     <row r="47" ht="11" customHeight="true" outlineLevel="3">
@@ -1852,7 +1858,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="11" t="n">
-        <v>772</v>
+        <v>730</v>
       </c>
     </row>
     <row r="48" ht="22" customHeight="true" outlineLevel="3">
@@ -1868,7 +1874,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="11" t="n">
-        <v>874</v>
+        <v>800</v>
       </c>
     </row>
     <row r="50" ht="11" customHeight="true" outlineLevel="3">
@@ -1884,7 +1890,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="11" t="n">
-        <v>918</v>
+        <v>773</v>
       </c>
     </row>
     <row r="52" ht="11" customHeight="true" outlineLevel="3">
@@ -1900,7 +1906,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="16" t="n">
-        <v>1278</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="54" ht="11" customHeight="true" outlineLevel="3">
@@ -1908,7 +1914,7 @@
         <v>53</v>
       </c>
       <c r="C54" s="11" t="n">
-        <v>538</v>
+        <v>454</v>
       </c>
     </row>
     <row r="55" ht="11" customHeight="true" outlineLevel="2">
@@ -1916,7 +1922,7 @@
         <v>54</v>
       </c>
       <c r="C55" s="12" t="n">
-        <v>40035</v>
+        <v>37941</v>
       </c>
     </row>
     <row r="56" ht="11" customHeight="true" outlineLevel="3">
@@ -1924,7 +1930,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="11" t="n">
-        <v>586</v>
+        <v>536</v>
       </c>
     </row>
     <row r="57" ht="11" customHeight="true" outlineLevel="3">
@@ -1932,7 +1938,7 @@
         <v>56</v>
       </c>
       <c r="C57" s="16" t="n">
-        <v>1449</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="58" ht="11" customHeight="true" outlineLevel="3">
@@ -1940,7 +1946,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="16" t="n">
-        <v>1669</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="59" ht="11" customHeight="true" outlineLevel="3">
@@ -1948,7 +1954,7 @@
         <v>58</v>
       </c>
       <c r="C59" s="16" t="n">
-        <v>2099</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="60" ht="11" customHeight="true" outlineLevel="3">
@@ -1956,7 +1962,7 @@
         <v>59</v>
       </c>
       <c r="C60" s="16" t="n">
-        <v>3979</v>
+        <v>3679</v>
       </c>
     </row>
     <row r="61" ht="11" customHeight="true" outlineLevel="3">
@@ -1964,7 +1970,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="16" t="n">
-        <v>1236</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="62" ht="11" customHeight="true" outlineLevel="3">
@@ -1972,7 +1978,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="16" t="n">
-        <v>2198</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="63" ht="11" customHeight="true" outlineLevel="3">
@@ -1980,7 +1986,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="16" t="n">
-        <v>1605</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="64" ht="11" customHeight="true" outlineLevel="3">
@@ -1988,7 +1994,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="16" t="n">
-        <v>1787</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="65" ht="11" customHeight="true" outlineLevel="3">
@@ -1996,7 +2002,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="16" t="n">
-        <v>2929</v>
+        <v>2771</v>
       </c>
     </row>
     <row r="66" ht="11" customHeight="true" outlineLevel="3">
@@ -2004,7 +2010,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="16" t="n">
-        <v>19041</v>
+        <v>18042</v>
       </c>
     </row>
     <row r="67" ht="11" customHeight="true" outlineLevel="3">
@@ -2012,7 +2018,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="11" t="n">
-        <v>842</v>
+        <v>749</v>
       </c>
     </row>
     <row r="68" ht="11" customHeight="true" outlineLevel="3">
@@ -2028,7 +2034,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="11" t="n">
-        <v>408</v>
+        <v>395</v>
       </c>
     </row>
     <row r="70" ht="11" customHeight="true" outlineLevel="3">
@@ -2044,7 +2050,7 @@
         <v>70</v>
       </c>
       <c r="C71" s="12" t="n">
-        <v>470142</v>
+        <v>446946</v>
       </c>
     </row>
     <row r="72" ht="11" customHeight="true" outlineLevel="2">
@@ -2052,7 +2058,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="12" t="n">
-        <v>131102</v>
+        <v>130437</v>
       </c>
     </row>
     <row r="73" ht="22" customHeight="true" outlineLevel="3">
@@ -2060,7 +2066,7 @@
         <v>72</v>
       </c>
       <c r="C73" s="16" t="n">
-        <v>30048</v>
+        <v>29933</v>
       </c>
     </row>
     <row r="74" ht="22" customHeight="true" outlineLevel="3">
@@ -2068,7 +2074,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="16" t="n">
-        <v>1530</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="75" ht="11" customHeight="true" outlineLevel="3">
@@ -2076,7 +2082,7 @@
         <v>74</v>
       </c>
       <c r="C75" s="16" t="n">
-        <v>13053</v>
+        <v>12668</v>
       </c>
     </row>
     <row r="76" ht="11" customHeight="true" outlineLevel="3">
@@ -2084,7 +2090,7 @@
         <v>75</v>
       </c>
       <c r="C76" s="16" t="n">
-        <v>2250</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="77" ht="11" customHeight="true" outlineLevel="3">
@@ -2092,7 +2098,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="16" t="n">
-        <v>2250</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="78" ht="22" customHeight="true" outlineLevel="3">
@@ -2100,7 +2106,7 @@
         <v>77</v>
       </c>
       <c r="C78" s="16" t="n">
-        <v>5220</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="79" ht="11" customHeight="true" outlineLevel="3">
@@ -2108,7 +2114,7 @@
         <v>78</v>
       </c>
       <c r="C79" s="16" t="n">
-        <v>12443</v>
+        <v>12123</v>
       </c>
     </row>
     <row r="80" ht="22" customHeight="true" outlineLevel="3">
@@ -2116,7 +2122,7 @@
         <v>79</v>
       </c>
       <c r="C80" s="16" t="n">
-        <v>1530</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="81" ht="22" customHeight="true" outlineLevel="3">
@@ -2124,7 +2130,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="16" t="n">
-        <v>22491</v>
+        <v>22266</v>
       </c>
     </row>
     <row r="82" ht="22" customHeight="true" outlineLevel="3">
@@ -2132,7 +2138,7 @@
         <v>81</v>
       </c>
       <c r="C82" s="16" t="n">
-        <v>5220</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="83" ht="22" customHeight="true" outlineLevel="3">
@@ -2140,7 +2146,7 @@
         <v>82</v>
       </c>
       <c r="C83" s="16" t="n">
-        <v>2250</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="84" ht="22" customHeight="true" outlineLevel="3">
@@ -2148,7 +2154,7 @@
         <v>83</v>
       </c>
       <c r="C84" s="16" t="n">
-        <v>2250</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="85" ht="11" customHeight="true" outlineLevel="3">
@@ -2156,7 +2162,7 @@
         <v>84</v>
       </c>
       <c r="C85" s="16" t="n">
-        <v>15170</v>
+        <v>14973</v>
       </c>
     </row>
     <row r="86" ht="11" customHeight="true" outlineLevel="3">
@@ -2164,7 +2170,7 @@
         <v>85</v>
       </c>
       <c r="C86" s="16" t="n">
-        <v>15397</v>
+        <v>15074</v>
       </c>
     </row>
     <row r="87" ht="11" customHeight="true" outlineLevel="2">
@@ -2172,7 +2178,7 @@
         <v>86</v>
       </c>
       <c r="C87" s="12" t="n">
-        <v>6574</v>
+        <v>4799</v>
       </c>
     </row>
     <row r="88" ht="11" customHeight="true" outlineLevel="3">
@@ -2180,7 +2186,7 @@
         <v>87</v>
       </c>
       <c r="C88" s="11" t="n">
-        <v>853</v>
+        <v>504</v>
       </c>
     </row>
     <row r="89" ht="11" customHeight="true" outlineLevel="3">
@@ -2196,7 +2202,7 @@
         <v>89</v>
       </c>
       <c r="C90" s="11" t="n">
-        <v>386</v>
+        <v>41</v>
       </c>
     </row>
     <row r="91" ht="11" customHeight="true" outlineLevel="3">
@@ -2204,7 +2210,7 @@
         <v>90</v>
       </c>
       <c r="C91" s="16" t="n">
-        <v>1341</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="92" ht="11" customHeight="true" outlineLevel="3">
@@ -2212,7 +2218,7 @@
         <v>91</v>
       </c>
       <c r="C92" s="11" t="n">
-        <v>419</v>
+        <v>340</v>
       </c>
     </row>
     <row r="93" ht="11" customHeight="true" outlineLevel="3">
@@ -2228,7 +2234,7 @@
         <v>93</v>
       </c>
       <c r="C94" s="16" t="n">
-        <v>1362</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="95" ht="11" customHeight="true" outlineLevel="3">
@@ -2236,7 +2242,7 @@
         <v>94</v>
       </c>
       <c r="C95" s="16" t="n">
-        <v>1438</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="96" ht="11" customHeight="true" outlineLevel="3">
@@ -2244,7 +2250,7 @@
         <v>95</v>
       </c>
       <c r="C96" s="11" t="n">
-        <v>130</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" ht="11" customHeight="true" outlineLevel="3">
@@ -2252,7 +2258,7 @@
         <v>96</v>
       </c>
       <c r="C97" s="11" t="n">
-        <v>310</v>
+        <v>297</v>
       </c>
     </row>
     <row r="98" ht="11" customHeight="true" outlineLevel="3">
@@ -2260,7 +2266,7 @@
         <v>97</v>
       </c>
       <c r="C98" s="11" t="n">
-        <v>269</v>
+        <v>139</v>
       </c>
     </row>
     <row r="99" ht="11" customHeight="true" outlineLevel="2">
@@ -2268,7 +2274,7 @@
         <v>98</v>
       </c>
       <c r="C99" s="12" t="n">
-        <v>41612</v>
+        <v>39279</v>
       </c>
     </row>
     <row r="100" ht="11" customHeight="true" outlineLevel="3">
@@ -2276,7 +2282,7 @@
         <v>99</v>
       </c>
       <c r="C100" s="11" t="n">
-        <v>333</v>
+        <v>301</v>
       </c>
     </row>
     <row r="101" ht="11" customHeight="true" outlineLevel="3">
@@ -2284,7 +2290,7 @@
         <v>100</v>
       </c>
       <c r="C101" s="11" t="n">
-        <v>240</v>
+        <v>191</v>
       </c>
     </row>
     <row r="102" ht="11" customHeight="true" outlineLevel="3">
@@ -2292,7 +2298,7 @@
         <v>101</v>
       </c>
       <c r="C102" s="16" t="n">
-        <v>1083</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="103" ht="11" customHeight="true" outlineLevel="3">
@@ -2308,7 +2314,7 @@
         <v>103</v>
       </c>
       <c r="C104" s="11" t="n">
-        <v>247</v>
+        <v>140</v>
       </c>
     </row>
     <row r="105" ht="11" customHeight="true" outlineLevel="3">
@@ -2316,7 +2322,7 @@
         <v>104</v>
       </c>
       <c r="C105" s="16" t="n">
-        <v>1354</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="106" ht="11" customHeight="true" outlineLevel="3">
@@ -2324,7 +2330,7 @@
         <v>105</v>
       </c>
       <c r="C106" s="16" t="n">
-        <v>4821</v>
+        <v>4471</v>
       </c>
     </row>
     <row r="107" ht="11" customHeight="true" outlineLevel="3">
@@ -2340,7 +2346,7 @@
         <v>107</v>
       </c>
       <c r="C108" s="16" t="n">
-        <v>15481</v>
+        <v>15106</v>
       </c>
     </row>
     <row r="109" ht="11" customHeight="true" outlineLevel="3">
@@ -2348,7 +2354,7 @@
         <v>108</v>
       </c>
       <c r="C109" s="16" t="n">
-        <v>5320</v>
+        <v>4970</v>
       </c>
     </row>
     <row r="110" ht="11" customHeight="true" outlineLevel="3">
@@ -2356,7 +2362,7 @@
         <v>109</v>
       </c>
       <c r="C110" s="11" t="n">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="111" ht="11" customHeight="true" outlineLevel="3">
@@ -2372,7 +2378,7 @@
         <v>111</v>
       </c>
       <c r="C112" s="11" t="n">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="113" ht="11" customHeight="true" outlineLevel="3">
@@ -2380,7 +2386,7 @@
         <v>112</v>
       </c>
       <c r="C113" s="11" t="n">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="114" ht="11" customHeight="true" outlineLevel="3">
@@ -2388,7 +2394,7 @@
         <v>113</v>
       </c>
       <c r="C114" s="11" t="n">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="115" ht="11" customHeight="true" outlineLevel="3">
@@ -2396,7 +2402,7 @@
         <v>114</v>
       </c>
       <c r="C115" s="11" t="n">
-        <v>712</v>
+        <v>542</v>
       </c>
     </row>
     <row r="116" ht="11" customHeight="true" outlineLevel="3">
@@ -2404,7 +2410,7 @@
         <v>115</v>
       </c>
       <c r="C116" s="11" t="n">
-        <v>479</v>
+        <v>412</v>
       </c>
     </row>
     <row r="117" ht="11" customHeight="true" outlineLevel="3">
@@ -2412,7 +2418,7 @@
         <v>116</v>
       </c>
       <c r="C117" s="11" t="n">
-        <v>809</v>
+        <v>625</v>
       </c>
     </row>
     <row r="118" ht="11" customHeight="true" outlineLevel="3">
@@ -2420,15 +2426,15 @@
         <v>117</v>
       </c>
       <c r="C118" s="11" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
     </row>
     <row r="119" ht="11" customHeight="true" outlineLevel="3">
       <c r="B119" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C119" s="16" t="n">
-        <v>3144</v>
+      <c r="C119" s="11" t="n">
+        <v>99</v>
       </c>
     </row>
     <row r="120" ht="11" customHeight="true" outlineLevel="3">
@@ -2436,7 +2442,7 @@
         <v>119</v>
       </c>
       <c r="C120" s="16" t="n">
-        <v>1237</v>
+        <v>2957</v>
       </c>
     </row>
     <row r="121" ht="11" customHeight="true" outlineLevel="3">
@@ -2444,7 +2450,7 @@
         <v>120</v>
       </c>
       <c r="C121" s="11" t="n">
-        <v>350</v>
+        <v>50</v>
       </c>
     </row>
     <row r="122" ht="11" customHeight="true" outlineLevel="3">
@@ -2460,15 +2466,15 @@
         <v>122</v>
       </c>
       <c r="C123" s="11" t="n">
-        <v>435</v>
+        <v>308</v>
       </c>
     </row>
     <row r="124" ht="11" customHeight="true" outlineLevel="3">
       <c r="B124" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C124" s="11" t="n">
-        <v>380</v>
+      <c r="C124" s="16" t="n">
+        <v>1092</v>
       </c>
     </row>
     <row r="125" ht="11" customHeight="true" outlineLevel="3">
@@ -2476,7 +2482,7 @@
         <v>124</v>
       </c>
       <c r="C125" s="11" t="n">
-        <v>64</v>
+        <v>407</v>
       </c>
     </row>
     <row r="126" ht="11" customHeight="true" outlineLevel="3">
@@ -2484,15 +2490,15 @@
         <v>125</v>
       </c>
       <c r="C126" s="11" t="n">
-        <v>85</v>
+        <v>351</v>
       </c>
     </row>
     <row r="127" ht="11" customHeight="true" outlineLevel="3">
       <c r="B127" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C127" s="16" t="n">
-        <v>1697</v>
+      <c r="C127" s="11" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="128" ht="11" customHeight="true" outlineLevel="3">
@@ -2500,15 +2506,15 @@
         <v>127</v>
       </c>
       <c r="C128" s="11" t="n">
-        <v>70</v>
+        <v>85</v>
       </c>
     </row>
     <row r="129" ht="11" customHeight="true" outlineLevel="3">
       <c r="B129" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="C129" s="11" t="n">
-        <v>591</v>
+      <c r="C129" s="16" t="n">
+        <v>1490</v>
       </c>
     </row>
     <row r="130" ht="11" customHeight="true" outlineLevel="3">
@@ -2516,15 +2522,15 @@
         <v>129</v>
       </c>
       <c r="C130" s="11" t="n">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="131" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B131" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="131" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B131" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C131" s="12" t="n">
-        <v>64466</v>
+      <c r="C131" s="11" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="132" ht="11" customHeight="true" outlineLevel="3">
@@ -2532,7 +2538,7 @@
         <v>131</v>
       </c>
       <c r="C132" s="11" t="n">
-        <v>60</v>
+        <v>504</v>
       </c>
     </row>
     <row r="133" ht="11" customHeight="true" outlineLevel="3">
@@ -2540,15 +2546,15 @@
         <v>132</v>
       </c>
       <c r="C133" s="11" t="n">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="134" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B134" s="15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="134" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B134" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="C134" s="11" t="n">
-        <v>358</v>
+      <c r="C134" s="12" t="n">
+        <v>60599</v>
       </c>
     </row>
     <row r="135" ht="11" customHeight="true" outlineLevel="3">
@@ -2556,7 +2562,7 @@
         <v>134</v>
       </c>
       <c r="C135" s="11" t="n">
-        <v>325</v>
+        <v>53</v>
       </c>
     </row>
     <row r="136" ht="11" customHeight="true" outlineLevel="3">
@@ -2564,7 +2570,7 @@
         <v>135</v>
       </c>
       <c r="C136" s="11" t="n">
-        <v>519</v>
+        <v>332</v>
       </c>
     </row>
     <row r="137" ht="11" customHeight="true" outlineLevel="3">
@@ -2572,7 +2578,7 @@
         <v>136</v>
       </c>
       <c r="C137" s="11" t="n">
-        <v>323</v>
+        <v>352</v>
       </c>
     </row>
     <row r="138" ht="11" customHeight="true" outlineLevel="3">
@@ -2580,7 +2586,7 @@
         <v>137</v>
       </c>
       <c r="C138" s="11" t="n">
-        <v>572</v>
+        <v>317</v>
       </c>
     </row>
     <row r="139" ht="11" customHeight="true" outlineLevel="3">
@@ -2588,15 +2594,15 @@
         <v>138</v>
       </c>
       <c r="C139" s="11" t="n">
-        <v>210</v>
+        <v>516</v>
       </c>
     </row>
     <row r="140" ht="11" customHeight="true" outlineLevel="3">
       <c r="B140" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="C140" s="16" t="n">
-        <v>1235</v>
+      <c r="C140" s="11" t="n">
+        <v>315</v>
       </c>
     </row>
     <row r="141" ht="11" customHeight="true" outlineLevel="3">
@@ -2604,7 +2610,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="11" t="n">
-        <v>375</v>
+        <v>563</v>
       </c>
     </row>
     <row r="142" ht="11" customHeight="true" outlineLevel="3">
@@ -2612,15 +2618,15 @@
         <v>141</v>
       </c>
       <c r="C142" s="11" t="n">
-        <v>108</v>
+        <v>202</v>
       </c>
     </row>
     <row r="143" ht="11" customHeight="true" outlineLevel="3">
       <c r="B143" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="C143" s="11" t="n">
-        <v>244</v>
+      <c r="C143" s="16" t="n">
+        <v>1229</v>
       </c>
     </row>
     <row r="144" ht="11" customHeight="true" outlineLevel="3">
@@ -2628,7 +2634,7 @@
         <v>143</v>
       </c>
       <c r="C144" s="11" t="n">
-        <v>527</v>
+        <v>375</v>
       </c>
     </row>
     <row r="145" ht="11" customHeight="true" outlineLevel="3">
@@ -2636,7 +2642,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="11" t="n">
-        <v>251</v>
+        <v>103</v>
       </c>
     </row>
     <row r="146" ht="11" customHeight="true" outlineLevel="3">
@@ -2644,7 +2650,7 @@
         <v>145</v>
       </c>
       <c r="C146" s="11" t="n">
-        <v>662</v>
+        <v>244</v>
       </c>
     </row>
     <row r="147" ht="11" customHeight="true" outlineLevel="3">
@@ -2652,15 +2658,15 @@
         <v>146</v>
       </c>
       <c r="C147" s="11" t="n">
-        <v>54</v>
+        <v>516</v>
       </c>
     </row>
     <row r="148" ht="11" customHeight="true" outlineLevel="3">
       <c r="B148" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C148" s="16" t="n">
-        <v>3313</v>
+      <c r="C148" s="11" t="n">
+        <v>248</v>
       </c>
     </row>
     <row r="149" ht="11" customHeight="true" outlineLevel="3">
@@ -2668,7 +2674,7 @@
         <v>148</v>
       </c>
       <c r="C149" s="11" t="n">
-        <v>424</v>
+        <v>659</v>
       </c>
     </row>
     <row r="150" ht="11" customHeight="true" outlineLevel="3">
@@ -2676,15 +2682,15 @@
         <v>149</v>
       </c>
       <c r="C150" s="11" t="n">
-        <v>224</v>
+        <v>54</v>
       </c>
     </row>
     <row r="151" ht="11" customHeight="true" outlineLevel="3">
       <c r="B151" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="C151" s="11" t="n">
-        <v>424</v>
+      <c r="C151" s="16" t="n">
+        <v>3162</v>
       </c>
     </row>
     <row r="152" ht="11" customHeight="true" outlineLevel="3">
@@ -2692,23 +2698,23 @@
         <v>151</v>
       </c>
       <c r="C152" s="11" t="n">
-        <v>45</v>
+        <v>342</v>
       </c>
     </row>
     <row r="153" ht="11" customHeight="true" outlineLevel="3">
       <c r="B153" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="C153" s="16" t="n">
-        <v>3480</v>
+      <c r="C153" s="11" t="n">
+        <v>211</v>
       </c>
     </row>
     <row r="154" ht="11" customHeight="true" outlineLevel="3">
       <c r="B154" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="C154" s="16" t="n">
-        <v>2372</v>
+      <c r="C154" s="11" t="n">
+        <v>342</v>
       </c>
     </row>
     <row r="155" ht="11" customHeight="true" outlineLevel="3">
@@ -2716,15 +2722,15 @@
         <v>154</v>
       </c>
       <c r="C155" s="11" t="n">
-        <v>396</v>
+        <v>42</v>
       </c>
     </row>
     <row r="156" ht="11" customHeight="true" outlineLevel="3">
       <c r="B156" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="C156" s="11" t="n">
-        <v>581</v>
+      <c r="C156" s="16" t="n">
+        <v>3312</v>
       </c>
     </row>
     <row r="157" ht="11" customHeight="true" outlineLevel="3">
@@ -2732,7 +2738,7 @@
         <v>156</v>
       </c>
       <c r="C157" s="16" t="n">
-        <v>2788</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="158" ht="11" customHeight="true" outlineLevel="3">
@@ -2740,7 +2746,7 @@
         <v>157</v>
       </c>
       <c r="C158" s="11" t="n">
-        <v>396</v>
+        <v>327</v>
       </c>
     </row>
     <row r="159" ht="11" customHeight="true" outlineLevel="3">
@@ -2748,7 +2754,7 @@
         <v>158</v>
       </c>
       <c r="C159" s="11" t="n">
-        <v>620</v>
+        <v>568</v>
       </c>
     </row>
     <row r="160" ht="11" customHeight="true" outlineLevel="3">
@@ -2756,7 +2762,7 @@
         <v>159</v>
       </c>
       <c r="C160" s="16" t="n">
-        <v>1226</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="161" ht="11" customHeight="true" outlineLevel="3">
@@ -2764,15 +2770,15 @@
         <v>160</v>
       </c>
       <c r="C161" s="11" t="n">
-        <v>56</v>
+        <v>327</v>
       </c>
     </row>
     <row r="162" ht="11" customHeight="true" outlineLevel="3">
       <c r="B162" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="C162" s="16" t="n">
-        <v>1346</v>
+      <c r="C162" s="11" t="n">
+        <v>604</v>
       </c>
     </row>
     <row r="163" ht="11" customHeight="true" outlineLevel="3">
@@ -2780,7 +2786,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="11" t="n">
-        <v>84</v>
+        <v>940</v>
       </c>
     </row>
     <row r="164" ht="11" customHeight="true" outlineLevel="3">
@@ -2788,15 +2794,15 @@
         <v>163</v>
       </c>
       <c r="C164" s="11" t="n">
-        <v>459</v>
+        <v>30</v>
       </c>
     </row>
     <row r="165" ht="11" customHeight="true" outlineLevel="3">
       <c r="B165" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="C165" s="11" t="n">
-        <v>591</v>
+      <c r="C165" s="16" t="n">
+        <v>1045</v>
       </c>
     </row>
     <row r="166" ht="11" customHeight="true" outlineLevel="3">
@@ -2804,15 +2810,15 @@
         <v>165</v>
       </c>
       <c r="C166" s="11" t="n">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="167" ht="11" customHeight="true" outlineLevel="3">
       <c r="B167" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="C167" s="16" t="n">
-        <v>3429</v>
+      <c r="C167" s="11" t="n">
+        <v>446</v>
       </c>
     </row>
     <row r="168" ht="11" customHeight="true" outlineLevel="3">
@@ -2820,7 +2826,7 @@
         <v>167</v>
       </c>
       <c r="C168" s="11" t="n">
-        <v>424</v>
+        <v>539</v>
       </c>
     </row>
     <row r="169" ht="11" customHeight="true" outlineLevel="3">
@@ -2828,7 +2834,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="11" t="n">
-        <v>274</v>
+        <v>31</v>
       </c>
     </row>
     <row r="170" ht="11" customHeight="true" outlineLevel="3">
@@ -2836,15 +2842,15 @@
         <v>169</v>
       </c>
       <c r="C170" s="16" t="n">
-        <v>1247</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="171" ht="11" customHeight="true" outlineLevel="3">
       <c r="B171" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C171" s="16" t="n">
-        <v>1057</v>
+      <c r="C171" s="11" t="n">
+        <v>342</v>
       </c>
     </row>
     <row r="172" ht="11" customHeight="true" outlineLevel="3">
@@ -2852,23 +2858,23 @@
         <v>171</v>
       </c>
       <c r="C172" s="11" t="n">
-        <v>56</v>
+        <v>261</v>
       </c>
     </row>
     <row r="173" ht="11" customHeight="true" outlineLevel="3">
       <c r="B173" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="C173" s="11" t="n">
-        <v>273</v>
+      <c r="C173" s="16" t="n">
+        <v>1218</v>
       </c>
     </row>
     <row r="174" ht="11" customHeight="true" outlineLevel="3">
       <c r="B174" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="C174" s="16" t="n">
-        <v>2801</v>
+      <c r="C174" s="11" t="n">
+        <v>779</v>
       </c>
     </row>
     <row r="175" ht="11" customHeight="true" outlineLevel="3">
@@ -2876,7 +2882,7 @@
         <v>174</v>
       </c>
       <c r="C175" s="11" t="n">
-        <v>424</v>
+        <v>30</v>
       </c>
     </row>
     <row r="176" ht="11" customHeight="true" outlineLevel="3">
@@ -2884,15 +2890,15 @@
         <v>175</v>
       </c>
       <c r="C176" s="11" t="n">
-        <v>147</v>
+        <v>260</v>
       </c>
     </row>
     <row r="177" ht="11" customHeight="true" outlineLevel="3">
       <c r="B177" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="C177" s="11" t="n">
-        <v>348</v>
+      <c r="C177" s="16" t="n">
+        <v>2661</v>
       </c>
     </row>
     <row r="178" ht="11" customHeight="true" outlineLevel="3">
@@ -2900,7 +2906,7 @@
         <v>177</v>
       </c>
       <c r="C178" s="11" t="n">
-        <v>56</v>
+        <v>342</v>
       </c>
     </row>
     <row r="179" ht="11" customHeight="true" outlineLevel="3">
@@ -2908,15 +2914,15 @@
         <v>178</v>
       </c>
       <c r="C179" s="11" t="n">
-        <v>98</v>
+        <v>131</v>
       </c>
     </row>
     <row r="180" ht="11" customHeight="true" outlineLevel="3">
       <c r="B180" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="C180" s="16" t="n">
-        <v>3024</v>
+      <c r="C180" s="11" t="n">
+        <v>277</v>
       </c>
     </row>
     <row r="181" ht="11" customHeight="true" outlineLevel="3">
@@ -2924,7 +2930,7 @@
         <v>180</v>
       </c>
       <c r="C181" s="11" t="n">
-        <v>424</v>
+        <v>30</v>
       </c>
     </row>
     <row r="182" ht="11" customHeight="true" outlineLevel="3">
@@ -2932,15 +2938,15 @@
         <v>181</v>
       </c>
       <c r="C182" s="11" t="n">
-        <v>210</v>
+        <v>85</v>
       </c>
     </row>
     <row r="183" ht="11" customHeight="true" outlineLevel="3">
       <c r="B183" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="C183" s="11" t="n">
-        <v>599</v>
+      <c r="C183" s="16" t="n">
+        <v>3132</v>
       </c>
     </row>
     <row r="184" ht="11" customHeight="true" outlineLevel="3">
@@ -2948,7 +2954,7 @@
         <v>183</v>
       </c>
       <c r="C184" s="11" t="n">
-        <v>84</v>
+        <v>342</v>
       </c>
     </row>
     <row r="185" ht="11" customHeight="true" outlineLevel="3">
@@ -2956,7 +2962,7 @@
         <v>184</v>
       </c>
       <c r="C185" s="11" t="n">
-        <v>219</v>
+        <v>194</v>
       </c>
     </row>
     <row r="186" ht="11" customHeight="true" outlineLevel="3">
@@ -2964,7 +2970,7 @@
         <v>185</v>
       </c>
       <c r="C186" s="11" t="n">
-        <v>386</v>
+        <v>501</v>
       </c>
     </row>
     <row r="187" ht="11" customHeight="true" outlineLevel="3">
@@ -2972,7 +2978,7 @@
         <v>186</v>
       </c>
       <c r="C187" s="11" t="n">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="188" ht="11" customHeight="true" outlineLevel="3">
@@ -2980,15 +2986,15 @@
         <v>187</v>
       </c>
       <c r="C188" s="11" t="n">
-        <v>293</v>
+        <v>206</v>
       </c>
     </row>
     <row r="189" ht="11" customHeight="true" outlineLevel="3">
       <c r="B189" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="C189" s="16" t="n">
-        <v>3427</v>
+      <c r="C189" s="11" t="n">
+        <v>451</v>
       </c>
     </row>
     <row r="190" ht="11" customHeight="true" outlineLevel="3">
@@ -2996,7 +3002,7 @@
         <v>189</v>
       </c>
       <c r="C190" s="11" t="n">
-        <v>424</v>
+        <v>30</v>
       </c>
     </row>
     <row r="191" ht="11" customHeight="true" outlineLevel="3">
@@ -3004,7 +3010,7 @@
         <v>190</v>
       </c>
       <c r="C191" s="11" t="n">
-        <v>110</v>
+        <v>280</v>
       </c>
     </row>
     <row r="192" ht="11" customHeight="true" outlineLevel="3">
@@ -3012,7 +3018,7 @@
         <v>191</v>
       </c>
       <c r="C192" s="16" t="n">
-        <v>1319</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="193" ht="11" customHeight="true" outlineLevel="3">
@@ -3020,7 +3026,7 @@
         <v>192</v>
       </c>
       <c r="C193" s="11" t="n">
-        <v>90</v>
+        <v>342</v>
       </c>
     </row>
     <row r="194" ht="11" customHeight="true" outlineLevel="3">
@@ -3028,7 +3034,7 @@
         <v>193</v>
       </c>
       <c r="C194" s="11" t="n">
-        <v>25</v>
+        <v>97</v>
       </c>
     </row>
     <row r="195" ht="11" customHeight="true" outlineLevel="3">
@@ -3036,7 +3042,7 @@
         <v>194</v>
       </c>
       <c r="C195" s="16" t="n">
-        <v>3272</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="196" ht="11" customHeight="true" outlineLevel="3">
@@ -3044,7 +3050,7 @@
         <v>195</v>
       </c>
       <c r="C196" s="11" t="n">
-        <v>424</v>
+        <v>51</v>
       </c>
     </row>
     <row r="197" ht="11" customHeight="true" outlineLevel="3">
@@ -3052,7 +3058,7 @@
         <v>196</v>
       </c>
       <c r="C197" s="11" t="n">
-        <v>160</v>
+        <v>12</v>
       </c>
     </row>
     <row r="198" ht="11" customHeight="true" outlineLevel="3">
@@ -3060,7 +3066,7 @@
         <v>197</v>
       </c>
       <c r="C198" s="16" t="n">
-        <v>1509</v>
+        <v>3094</v>
       </c>
     </row>
     <row r="199" ht="11" customHeight="true" outlineLevel="3">
@@ -3068,7 +3074,7 @@
         <v>198</v>
       </c>
       <c r="C199" s="11" t="n">
-        <v>56</v>
+        <v>342</v>
       </c>
     </row>
     <row r="200" ht="11" customHeight="true" outlineLevel="3">
@@ -3076,7 +3082,7 @@
         <v>199</v>
       </c>
       <c r="C200" s="11" t="n">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="201" ht="11" customHeight="true" outlineLevel="3">
@@ -3084,7 +3090,7 @@
         <v>200</v>
       </c>
       <c r="C201" s="16" t="n">
-        <v>2816</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="202" ht="11" customHeight="true" outlineLevel="3">
@@ -3092,7 +3098,7 @@
         <v>201</v>
       </c>
       <c r="C202" s="11" t="n">
-        <v>396</v>
+        <v>30</v>
       </c>
     </row>
     <row r="203" ht="11" customHeight="true" outlineLevel="3">
@@ -3100,15 +3106,15 @@
         <v>202</v>
       </c>
       <c r="C203" s="11" t="n">
-        <v>186</v>
+        <v>100</v>
       </c>
     </row>
     <row r="204" ht="11" customHeight="true" outlineLevel="3">
       <c r="B204" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="C204" s="11" t="n">
-        <v>25</v>
+      <c r="C204" s="16" t="n">
+        <v>2841</v>
       </c>
     </row>
     <row r="205" ht="11" customHeight="true" outlineLevel="3">
@@ -3116,7 +3122,7 @@
         <v>204</v>
       </c>
       <c r="C205" s="11" t="n">
-        <v>484</v>
+        <v>327</v>
       </c>
     </row>
     <row r="206" ht="11" customHeight="true" outlineLevel="3">
@@ -3124,15 +3130,15 @@
         <v>205</v>
       </c>
       <c r="C206" s="11" t="n">
-        <v>333</v>
+        <v>173</v>
       </c>
     </row>
     <row r="207" ht="11" customHeight="true" outlineLevel="3">
       <c r="B207" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C207" s="16" t="n">
-        <v>2555</v>
+      <c r="C207" s="11" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="208" ht="11" customHeight="true" outlineLevel="3">
@@ -3140,23 +3146,23 @@
         <v>207</v>
       </c>
       <c r="C208" s="11" t="n">
-        <v>253</v>
+        <v>479</v>
       </c>
     </row>
     <row r="209" ht="11" customHeight="true" outlineLevel="3">
       <c r="B209" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="C209" s="16" t="n">
-        <v>1023</v>
+      <c r="C209" s="11" t="n">
+        <v>333</v>
       </c>
     </row>
     <row r="210" ht="11" customHeight="true" outlineLevel="3">
       <c r="B210" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="C210" s="11" t="n">
-        <v>459</v>
+      <c r="C210" s="16" t="n">
+        <v>2549</v>
       </c>
     </row>
     <row r="211" ht="11" customHeight="true" outlineLevel="3">
@@ -3171,8 +3177,8 @@
       <c r="B212" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="C212" s="11" t="n">
-        <v>317</v>
+      <c r="C212" s="16" t="n">
+        <v>1016</v>
       </c>
     </row>
     <row r="213" ht="11" customHeight="true" outlineLevel="3">
@@ -3180,31 +3186,31 @@
         <v>212</v>
       </c>
       <c r="C213" s="11" t="n">
-        <v>97</v>
+        <v>454</v>
       </c>
     </row>
     <row r="214" ht="11" customHeight="true" outlineLevel="3">
       <c r="B214" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="C214" s="16" t="n">
-        <v>1967</v>
+      <c r="C214" s="11" t="n">
+        <v>253</v>
       </c>
     </row>
     <row r="215" ht="11" customHeight="true" outlineLevel="3">
       <c r="B215" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="C215" s="16" t="n">
-        <v>1407</v>
-      </c>
-    </row>
-    <row r="216" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B216" s="14" t="s">
+      <c r="C215" s="11" t="n">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="216" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B216" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="C216" s="12" t="n">
-        <v>34340</v>
+      <c r="C216" s="11" t="n">
+        <v>97</v>
       </c>
     </row>
     <row r="217" ht="11" customHeight="true" outlineLevel="3">
@@ -3212,23 +3218,23 @@
         <v>216</v>
       </c>
       <c r="C217" s="16" t="n">
-        <v>1031</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="218" ht="11" customHeight="true" outlineLevel="3">
       <c r="B218" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="C218" s="11" t="n">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="219" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B219" s="15" t="s">
+      <c r="C218" s="16" t="n">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="219" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B219" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="C219" s="11" t="n">
-        <v>951</v>
+      <c r="C219" s="12" t="n">
+        <v>30989</v>
       </c>
     </row>
     <row r="220" ht="11" customHeight="true" outlineLevel="3">
@@ -3236,15 +3242,15 @@
         <v>219</v>
       </c>
       <c r="C220" s="11" t="n">
-        <v>506</v>
+        <v>987</v>
       </c>
     </row>
     <row r="221" ht="11" customHeight="true" outlineLevel="3">
       <c r="B221" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="C221" s="16" t="n">
-        <v>2809</v>
+      <c r="C221" s="11" t="n">
+        <v>359</v>
       </c>
     </row>
     <row r="222" ht="11" customHeight="true" outlineLevel="3">
@@ -3252,7 +3258,7 @@
         <v>221</v>
       </c>
       <c r="C222" s="11" t="n">
-        <v>44</v>
+        <v>834</v>
       </c>
     </row>
     <row r="223" ht="11" customHeight="true" outlineLevel="3">
@@ -3260,15 +3266,15 @@
         <v>222</v>
       </c>
       <c r="C223" s="11" t="n">
-        <v>91</v>
+        <v>432</v>
       </c>
     </row>
     <row r="224" ht="11" customHeight="true" outlineLevel="3">
       <c r="B224" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="C224" s="11" t="n">
-        <v>246</v>
+      <c r="C224" s="16" t="n">
+        <v>2559</v>
       </c>
     </row>
     <row r="225" ht="11" customHeight="true" outlineLevel="3">
@@ -3276,7 +3282,7 @@
         <v>224</v>
       </c>
       <c r="C225" s="11" t="n">
-        <v>386</v>
+        <v>44</v>
       </c>
     </row>
     <row r="226" ht="11" customHeight="true" outlineLevel="3">
@@ -3284,15 +3290,15 @@
         <v>225</v>
       </c>
       <c r="C226" s="11" t="n">
-        <v>742</v>
+        <v>86</v>
       </c>
     </row>
     <row r="227" ht="11" customHeight="true" outlineLevel="3">
       <c r="B227" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="C227" s="16" t="n">
-        <v>1130</v>
+      <c r="C227" s="11" t="n">
+        <v>235</v>
       </c>
     </row>
     <row r="228" ht="11" customHeight="true" outlineLevel="3">
@@ -3300,7 +3306,7 @@
         <v>227</v>
       </c>
       <c r="C228" s="11" t="n">
-        <v>937</v>
+        <v>357</v>
       </c>
     </row>
     <row r="229" ht="11" customHeight="true" outlineLevel="3">
@@ -3308,15 +3314,15 @@
         <v>228</v>
       </c>
       <c r="C229" s="11" t="n">
-        <v>680</v>
+        <v>733</v>
       </c>
     </row>
     <row r="230" ht="11" customHeight="true" outlineLevel="3">
       <c r="B230" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C230" s="11" t="n">
-        <v>592</v>
+      <c r="C230" s="16" t="n">
+        <v>1035</v>
       </c>
     </row>
     <row r="231" ht="11" customHeight="true" outlineLevel="3">
@@ -3324,7 +3330,7 @@
         <v>230</v>
       </c>
       <c r="C231" s="11" t="n">
-        <v>250</v>
+        <v>759</v>
       </c>
     </row>
     <row r="232" ht="11" customHeight="true" outlineLevel="3">
@@ -3332,7 +3338,7 @@
         <v>231</v>
       </c>
       <c r="C232" s="11" t="n">
-        <v>175</v>
+        <v>595</v>
       </c>
     </row>
     <row r="233" ht="11" customHeight="true" outlineLevel="3">
@@ -3340,7 +3346,7 @@
         <v>232</v>
       </c>
       <c r="C233" s="11" t="n">
-        <v>576</v>
+        <v>468</v>
       </c>
     </row>
     <row r="234" ht="11" customHeight="true" outlineLevel="3">
@@ -3348,7 +3354,7 @@
         <v>233</v>
       </c>
       <c r="C234" s="11" t="n">
-        <v>884</v>
+        <v>190</v>
       </c>
     </row>
     <row r="235" ht="11" customHeight="true" outlineLevel="3">
@@ -3356,7 +3362,7 @@
         <v>234</v>
       </c>
       <c r="C235" s="11" t="n">
-        <v>458</v>
+        <v>164</v>
       </c>
     </row>
     <row r="236" ht="11" customHeight="true" outlineLevel="3">
@@ -3364,39 +3370,39 @@
         <v>235</v>
       </c>
       <c r="C236" s="11" t="n">
-        <v>981</v>
+        <v>546</v>
       </c>
     </row>
     <row r="237" ht="11" customHeight="true" outlineLevel="3">
       <c r="B237" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="C237" s="16" t="n">
-        <v>1006</v>
+      <c r="C237" s="11" t="n">
+        <v>843</v>
       </c>
     </row>
     <row r="238" ht="11" customHeight="true" outlineLevel="3">
       <c r="B238" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="C238" s="16" t="n">
-        <v>2718</v>
+      <c r="C238" s="11" t="n">
+        <v>262</v>
       </c>
     </row>
     <row r="239" ht="11" customHeight="true" outlineLevel="3">
       <c r="B239" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="C239" s="16" t="n">
-        <v>1146</v>
+      <c r="C239" s="11" t="n">
+        <v>866</v>
       </c>
     </row>
     <row r="240" ht="11" customHeight="true" outlineLevel="3">
       <c r="B240" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="C240" s="16" t="n">
-        <v>1418</v>
+      <c r="C240" s="11" t="n">
+        <v>894</v>
       </c>
     </row>
     <row r="241" ht="11" customHeight="true" outlineLevel="3">
@@ -3404,7 +3410,7 @@
         <v>240</v>
       </c>
       <c r="C241" s="16" t="n">
-        <v>1891</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="242" ht="11" customHeight="true" outlineLevel="3">
@@ -3412,7 +3418,7 @@
         <v>241</v>
       </c>
       <c r="C242" s="16" t="n">
-        <v>1516</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="243" ht="11" customHeight="true" outlineLevel="3">
@@ -3420,7 +3426,7 @@
         <v>242</v>
       </c>
       <c r="C243" s="16" t="n">
-        <v>1811</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="244" ht="11" customHeight="true" outlineLevel="3">
@@ -3428,7 +3434,7 @@
         <v>243</v>
       </c>
       <c r="C244" s="16" t="n">
-        <v>1276</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="245" ht="11" customHeight="true" outlineLevel="3">
@@ -3436,7 +3442,7 @@
         <v>244</v>
       </c>
       <c r="C245" s="16" t="n">
-        <v>2405</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="246" ht="11" customHeight="true" outlineLevel="3">
@@ -3444,7 +3450,7 @@
         <v>245</v>
       </c>
       <c r="C246" s="16" t="n">
-        <v>1247</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="247" ht="11" customHeight="true" outlineLevel="3">
@@ -3452,31 +3458,31 @@
         <v>246</v>
       </c>
       <c r="C247" s="16" t="n">
-        <v>3090</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="248" ht="11" customHeight="true" outlineLevel="3">
       <c r="B248" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="C248" s="11" t="n">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="249" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B249" s="14" t="s">
+      <c r="C248" s="16" t="n">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="249" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B249" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="C249" s="12" t="n">
-        <v>5184</v>
+      <c r="C249" s="16" t="n">
+        <v>1181</v>
       </c>
     </row>
     <row r="250" ht="11" customHeight="true" outlineLevel="3">
       <c r="B250" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="C250" s="11" t="n">
-        <v>781</v>
+      <c r="C250" s="16" t="n">
+        <v>2899</v>
       </c>
     </row>
     <row r="251" ht="11" customHeight="true" outlineLevel="3">
@@ -3484,15 +3490,15 @@
         <v>250</v>
       </c>
       <c r="C251" s="11" t="n">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="252" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B252" s="15" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="252" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B252" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="C252" s="11" t="n">
-        <v>442</v>
+      <c r="C252" s="12" t="n">
+        <v>4209</v>
       </c>
     </row>
     <row r="253" ht="11" customHeight="true" outlineLevel="3">
@@ -3500,7 +3506,7 @@
         <v>252</v>
       </c>
       <c r="C253" s="11" t="n">
-        <v>192</v>
+        <v>579</v>
       </c>
     </row>
     <row r="254" ht="11" customHeight="true" outlineLevel="3">
@@ -3508,7 +3514,7 @@
         <v>253</v>
       </c>
       <c r="C254" s="11" t="n">
-        <v>240</v>
+        <v>687</v>
       </c>
     </row>
     <row r="255" ht="11" customHeight="true" outlineLevel="3">
@@ -3516,7 +3522,7 @@
         <v>254</v>
       </c>
       <c r="C255" s="11" t="n">
-        <v>283</v>
+        <v>370</v>
       </c>
     </row>
     <row r="256" ht="11" customHeight="true" outlineLevel="3">
@@ -3524,7 +3530,7 @@
         <v>255</v>
       </c>
       <c r="C256" s="11" t="n">
-        <v>10</v>
+        <v>192</v>
       </c>
     </row>
     <row r="257" ht="11" customHeight="true" outlineLevel="3">
@@ -3532,7 +3538,7 @@
         <v>256</v>
       </c>
       <c r="C257" s="11" t="n">
-        <v>26</v>
+        <v>157</v>
       </c>
     </row>
     <row r="258" ht="11" customHeight="true" outlineLevel="3">
@@ -3540,7 +3546,7 @@
         <v>257</v>
       </c>
       <c r="C258" s="11" t="n">
-        <v>754</v>
+        <v>277</v>
       </c>
     </row>
     <row r="259" ht="11" customHeight="true" outlineLevel="3">
@@ -3548,7 +3554,7 @@
         <v>258</v>
       </c>
       <c r="C259" s="11" t="n">
-        <v>321</v>
+        <v>10</v>
       </c>
     </row>
     <row r="260" ht="11" customHeight="true" outlineLevel="3">
@@ -3556,7 +3562,7 @@
         <v>259</v>
       </c>
       <c r="C260" s="11" t="n">
-        <v>279</v>
+        <v>24</v>
       </c>
     </row>
     <row r="261" ht="11" customHeight="true" outlineLevel="3">
@@ -3564,7 +3570,7 @@
         <v>260</v>
       </c>
       <c r="C261" s="11" t="n">
-        <v>257</v>
+        <v>609</v>
       </c>
     </row>
     <row r="262" ht="11" customHeight="true" outlineLevel="3">
@@ -3572,7 +3578,7 @@
         <v>261</v>
       </c>
       <c r="C262" s="11" t="n">
-        <v>268</v>
+        <v>238</v>
       </c>
     </row>
     <row r="263" ht="11" customHeight="true" outlineLevel="3">
@@ -3580,7 +3586,7 @@
         <v>262</v>
       </c>
       <c r="C263" s="11" t="n">
-        <v>248</v>
+        <v>194</v>
       </c>
     </row>
     <row r="264" ht="11" customHeight="true" outlineLevel="3">
@@ -3588,7 +3594,7 @@
         <v>263</v>
       </c>
       <c r="C264" s="11" t="n">
-        <v>148</v>
+        <v>121</v>
       </c>
     </row>
     <row r="265" ht="11" customHeight="true" outlineLevel="3">
@@ -3596,7 +3602,7 @@
         <v>264</v>
       </c>
       <c r="C265" s="11" t="n">
-        <v>10</v>
+        <v>226</v>
       </c>
     </row>
     <row r="266" ht="11" customHeight="true" outlineLevel="3">
@@ -3604,55 +3610,55 @@
         <v>265</v>
       </c>
       <c r="C266" s="11" t="n">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="267" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B267" s="14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="267" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B267" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="C267" s="12" t="n">
-        <v>29983</v>
-      </c>
-    </row>
-    <row r="268" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C267" s="11" t="n">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="268" ht="11" customHeight="true" outlineLevel="3">
       <c r="B268" s="15" t="s">
         <v>267</v>
       </c>
       <c r="C268" s="11" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="269" ht="22" customHeight="true" outlineLevel="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="269" ht="11" customHeight="true" outlineLevel="3">
       <c r="B269" s="15" t="s">
         <v>268</v>
       </c>
       <c r="C269" s="11" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="270" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B270" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="270" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B270" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="C270" s="11" t="n">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="271" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C270" s="12" t="n">
+        <v>27820</v>
+      </c>
+    </row>
+    <row r="271" ht="22" customHeight="true" outlineLevel="3">
       <c r="B271" s="15" t="s">
         <v>270</v>
       </c>
       <c r="C271" s="11" t="n">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="272" ht="11" customHeight="true" outlineLevel="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="272" ht="22" customHeight="true" outlineLevel="3">
       <c r="B272" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="C272" s="16" t="n">
-        <v>1368</v>
+      <c r="C272" s="11" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="273" ht="11" customHeight="true" outlineLevel="3">
@@ -3660,7 +3666,7 @@
         <v>272</v>
       </c>
       <c r="C273" s="11" t="n">
-        <v>834</v>
+        <v>146</v>
       </c>
     </row>
     <row r="274" ht="11" customHeight="true" outlineLevel="3">
@@ -3668,39 +3674,39 @@
         <v>273</v>
       </c>
       <c r="C274" s="11" t="n">
-        <v>629</v>
+        <v>169</v>
       </c>
     </row>
     <row r="275" ht="11" customHeight="true" outlineLevel="3">
       <c r="B275" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="C275" s="11" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="276" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C275" s="16" t="n">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="276" ht="11" customHeight="true" outlineLevel="3">
       <c r="B276" s="15" t="s">
         <v>275</v>
       </c>
       <c r="C276" s="11" t="n">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="277" ht="22" customHeight="true" outlineLevel="3">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="277" ht="11" customHeight="true" outlineLevel="3">
       <c r="B277" s="15" t="s">
         <v>276</v>
       </c>
       <c r="C277" s="11" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="278" ht="22" customHeight="true" outlineLevel="3">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="278" ht="11" customHeight="true" outlineLevel="3">
       <c r="B278" s="15" t="s">
         <v>277</v>
       </c>
       <c r="C278" s="11" t="n">
-        <v>203</v>
+        <v>70</v>
       </c>
     </row>
     <row r="279" ht="22" customHeight="true" outlineLevel="3">
@@ -3708,7 +3714,7 @@
         <v>278</v>
       </c>
       <c r="C279" s="11" t="n">
-        <v>57</v>
+        <v>432</v>
       </c>
     </row>
     <row r="280" ht="22" customHeight="true" outlineLevel="3">
@@ -3716,7 +3722,7 @@
         <v>279</v>
       </c>
       <c r="C280" s="11" t="n">
-        <v>756</v>
+        <v>37</v>
       </c>
     </row>
     <row r="281" ht="22" customHeight="true" outlineLevel="3">
@@ -3724,7 +3730,7 @@
         <v>280</v>
       </c>
       <c r="C281" s="11" t="n">
-        <v>41</v>
+        <v>193</v>
       </c>
     </row>
     <row r="282" ht="22" customHeight="true" outlineLevel="3">
@@ -3732,7 +3738,7 @@
         <v>281</v>
       </c>
       <c r="C282" s="11" t="n">
-        <v>379</v>
+        <v>54</v>
       </c>
     </row>
     <row r="283" ht="22" customHeight="true" outlineLevel="3">
@@ -3740,7 +3746,7 @@
         <v>282</v>
       </c>
       <c r="C283" s="11" t="n">
-        <v>70</v>
+        <v>641</v>
       </c>
     </row>
     <row r="284" ht="22" customHeight="true" outlineLevel="3">
@@ -3748,31 +3754,31 @@
         <v>283</v>
       </c>
       <c r="C284" s="11" t="n">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="285" ht="11" customHeight="true" outlineLevel="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="285" ht="22" customHeight="true" outlineLevel="3">
       <c r="B285" s="15" t="s">
         <v>284</v>
       </c>
       <c r="C285" s="11" t="n">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="286" ht="11" customHeight="true" outlineLevel="3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="286" ht="22" customHeight="true" outlineLevel="3">
       <c r="B286" s="15" t="s">
         <v>285</v>
       </c>
       <c r="C286" s="11" t="n">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="287" ht="11" customHeight="true" outlineLevel="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="287" ht="22" customHeight="true" outlineLevel="3">
       <c r="B287" s="15" t="s">
         <v>286</v>
       </c>
       <c r="C287" s="11" t="n">
-        <v>70</v>
+        <v>157</v>
       </c>
     </row>
     <row r="288" ht="11" customHeight="true" outlineLevel="3">
@@ -3780,7 +3786,7 @@
         <v>287</v>
       </c>
       <c r="C288" s="11" t="n">
-        <v>349</v>
+        <v>560</v>
       </c>
     </row>
     <row r="289" ht="11" customHeight="true" outlineLevel="3">
@@ -3788,15 +3794,15 @@
         <v>288</v>
       </c>
       <c r="C289" s="11" t="n">
-        <v>282</v>
+        <v>671</v>
       </c>
     </row>
     <row r="290" ht="11" customHeight="true" outlineLevel="3">
       <c r="B290" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="C290" s="16" t="n">
-        <v>2947</v>
+      <c r="C290" s="11" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="291" ht="11" customHeight="true" outlineLevel="3">
@@ -3804,7 +3810,7 @@
         <v>290</v>
       </c>
       <c r="C291" s="11" t="n">
-        <v>851</v>
+        <v>339</v>
       </c>
     </row>
     <row r="292" ht="11" customHeight="true" outlineLevel="3">
@@ -3812,23 +3818,23 @@
         <v>291</v>
       </c>
       <c r="C292" s="11" t="n">
-        <v>364</v>
+        <v>272</v>
       </c>
     </row>
     <row r="293" ht="11" customHeight="true" outlineLevel="3">
       <c r="B293" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="C293" s="11" t="n">
-        <v>947</v>
+      <c r="C293" s="16" t="n">
+        <v>2888</v>
       </c>
     </row>
     <row r="294" ht="11" customHeight="true" outlineLevel="3">
       <c r="B294" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="C294" s="16" t="n">
-        <v>2118</v>
+      <c r="C294" s="11" t="n">
+        <v>781</v>
       </c>
     </row>
     <row r="295" ht="11" customHeight="true" outlineLevel="3">
@@ -3836,7 +3842,7 @@
         <v>294</v>
       </c>
       <c r="C295" s="11" t="n">
-        <v>70</v>
+        <v>352</v>
       </c>
     </row>
     <row r="296" ht="11" customHeight="true" outlineLevel="3">
@@ -3844,31 +3850,31 @@
         <v>295</v>
       </c>
       <c r="C296" s="11" t="n">
-        <v>5</v>
+        <v>883</v>
       </c>
     </row>
     <row r="297" ht="11" customHeight="true" outlineLevel="3">
       <c r="B297" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="C297" s="11" t="n">
-        <v>95</v>
+      <c r="C297" s="16" t="n">
+        <v>2045</v>
       </c>
     </row>
     <row r="298" ht="11" customHeight="true" outlineLevel="3">
       <c r="B298" s="15" t="s">
         <v>297</v>
       </c>
-      <c r="C298" s="16" t="n">
-        <v>2547</v>
+      <c r="C298" s="11" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="299" ht="11" customHeight="true" outlineLevel="3">
       <c r="B299" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="C299" s="16" t="n">
-        <v>8881</v>
+      <c r="C299" s="11" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="300" ht="11" customHeight="true" outlineLevel="3">
@@ -3876,7 +3882,7 @@
         <v>299</v>
       </c>
       <c r="C300" s="11" t="n">
-        <v>846</v>
+        <v>34</v>
       </c>
     </row>
     <row r="301" ht="11" customHeight="true" outlineLevel="3">
@@ -3884,95 +3890,95 @@
         <v>300</v>
       </c>
       <c r="C301" s="16" t="n">
-        <v>2533</v>
-      </c>
-    </row>
-    <row r="302" ht="22" customHeight="true" outlineLevel="3">
+        <v>2265</v>
+      </c>
+    </row>
+    <row r="302" ht="11" customHeight="true" outlineLevel="3">
       <c r="B302" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="C302" s="11" t="n">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="303" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C302" s="16" t="n">
+        <v>8283</v>
+      </c>
+    </row>
+    <row r="303" ht="11" customHeight="true" outlineLevel="3">
       <c r="B303" s="15" t="s">
         <v>302</v>
       </c>
       <c r="C303" s="11" t="n">
-        <v>1</v>
+        <v>846</v>
       </c>
     </row>
     <row r="304" ht="11" customHeight="true" outlineLevel="3">
       <c r="B304" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="C304" s="11" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="305" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C304" s="16" t="n">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="305" ht="22" customHeight="true" outlineLevel="3">
       <c r="B305" s="15" t="s">
         <v>304</v>
       </c>
       <c r="C305" s="11" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="306" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B306" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="306" ht="22" customHeight="true" outlineLevel="3">
+      <c r="B306" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="C306" s="12" t="n">
-        <v>32555</v>
+      <c r="C306" s="11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="307" ht="11" customHeight="true" outlineLevel="3">
       <c r="B307" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="C307" s="16" t="n">
-        <v>2295</v>
+      <c r="C307" s="11" t="n">
+        <v>169</v>
       </c>
     </row>
     <row r="308" ht="11" customHeight="true" outlineLevel="3">
       <c r="B308" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="C308" s="16" t="n">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="309" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B309" s="15" t="s">
+      <c r="C308" s="11" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="309" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B309" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="C309" s="16" t="n">
-        <v>2834</v>
+      <c r="C309" s="12" t="n">
+        <v>31018</v>
       </c>
     </row>
     <row r="310" ht="11" customHeight="true" outlineLevel="3">
       <c r="B310" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="C310" s="11" t="n">
-        <v>581</v>
+      <c r="C310" s="16" t="n">
+        <v>2169</v>
       </c>
     </row>
     <row r="311" ht="11" customHeight="true" outlineLevel="3">
       <c r="B311" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="C311" s="11" t="n">
-        <v>836</v>
+      <c r="C311" s="16" t="n">
+        <v>1338</v>
       </c>
     </row>
     <row r="312" ht="11" customHeight="true" outlineLevel="3">
       <c r="B312" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="C312" s="11" t="n">
-        <v>466</v>
+      <c r="C312" s="16" t="n">
+        <v>2706</v>
       </c>
     </row>
     <row r="313" ht="11" customHeight="true" outlineLevel="3">
@@ -3980,15 +3986,15 @@
         <v>312</v>
       </c>
       <c r="C313" s="11" t="n">
-        <v>224</v>
+        <v>554</v>
       </c>
     </row>
     <row r="314" ht="11" customHeight="true" outlineLevel="3">
       <c r="B314" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="C314" s="16" t="n">
-        <v>1065</v>
+      <c r="C314" s="11" t="n">
+        <v>809</v>
       </c>
     </row>
     <row r="315" ht="11" customHeight="true" outlineLevel="3">
@@ -3996,7 +4002,7 @@
         <v>314</v>
       </c>
       <c r="C315" s="11" t="n">
-        <v>860</v>
+        <v>445</v>
       </c>
     </row>
     <row r="316" ht="11" customHeight="true" outlineLevel="3">
@@ -4004,23 +4010,23 @@
         <v>315</v>
       </c>
       <c r="C316" s="11" t="n">
-        <v>457</v>
+        <v>224</v>
       </c>
     </row>
     <row r="317" ht="11" customHeight="true" outlineLevel="3">
       <c r="B317" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="C317" s="11" t="n">
-        <v>757</v>
+      <c r="C317" s="16" t="n">
+        <v>1002</v>
       </c>
     </row>
     <row r="318" ht="11" customHeight="true" outlineLevel="3">
       <c r="B318" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="C318" s="16" t="n">
-        <v>1019</v>
+      <c r="C318" s="11" t="n">
+        <v>775</v>
       </c>
     </row>
     <row r="319" ht="11" customHeight="true" outlineLevel="3">
@@ -4028,7 +4034,7 @@
         <v>318</v>
       </c>
       <c r="C319" s="11" t="n">
-        <v>320</v>
+        <v>435</v>
       </c>
     </row>
     <row r="320" ht="11" customHeight="true" outlineLevel="3">
@@ -4036,7 +4042,7 @@
         <v>319</v>
       </c>
       <c r="C320" s="11" t="n">
-        <v>282</v>
+        <v>711</v>
       </c>
     </row>
     <row r="321" ht="11" customHeight="true" outlineLevel="3">
@@ -4044,7 +4050,7 @@
         <v>320</v>
       </c>
       <c r="C321" s="11" t="n">
-        <v>233</v>
+        <v>977</v>
       </c>
     </row>
     <row r="322" ht="11" customHeight="true" outlineLevel="3">
@@ -4052,15 +4058,15 @@
         <v>321</v>
       </c>
       <c r="C322" s="11" t="n">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="323" ht="22" customHeight="true" outlineLevel="3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="323" ht="11" customHeight="true" outlineLevel="3">
       <c r="B323" s="15" t="s">
         <v>322</v>
       </c>
       <c r="C323" s="11" t="n">
-        <v>187</v>
+        <v>239</v>
       </c>
     </row>
     <row r="324" ht="11" customHeight="true" outlineLevel="3">
@@ -4068,7 +4074,7 @@
         <v>323</v>
       </c>
       <c r="C324" s="11" t="n">
-        <v>194</v>
+        <v>181</v>
       </c>
     </row>
     <row r="325" ht="11" customHeight="true" outlineLevel="3">
@@ -4076,7 +4082,7 @@
         <v>324</v>
       </c>
       <c r="C325" s="11" t="n">
-        <v>217</v>
+        <v>246</v>
       </c>
     </row>
     <row r="326" ht="22" customHeight="true" outlineLevel="3">
@@ -4084,15 +4090,15 @@
         <v>325</v>
       </c>
       <c r="C326" s="11" t="n">
-        <v>234</v>
+        <v>164</v>
       </c>
     </row>
     <row r="327" ht="11" customHeight="true" outlineLevel="3">
       <c r="B327" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="C327" s="16" t="n">
-        <v>10264</v>
+      <c r="C327" s="11" t="n">
+        <v>188</v>
       </c>
     </row>
     <row r="328" ht="11" customHeight="true" outlineLevel="3">
@@ -4100,15 +4106,15 @@
         <v>327</v>
       </c>
       <c r="C328" s="11" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="329" ht="11" customHeight="true" outlineLevel="3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="329" ht="22" customHeight="true" outlineLevel="3">
       <c r="B329" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="C329" s="16" t="n">
-        <v>4776</v>
+      <c r="C329" s="11" t="n">
+        <v>211</v>
       </c>
     </row>
     <row r="330" ht="11" customHeight="true" outlineLevel="3">
@@ -4116,7 +4122,7 @@
         <v>329</v>
       </c>
       <c r="C330" s="16" t="n">
-        <v>1828</v>
+        <v>9980</v>
       </c>
     </row>
     <row r="331" ht="11" customHeight="true" outlineLevel="3">
@@ -4124,23 +4130,23 @@
         <v>330</v>
       </c>
       <c r="C331" s="11" t="n">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="332" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B332" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="332" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B332" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="C332" s="12" t="n">
-        <v>2155</v>
+      <c r="C332" s="16" t="n">
+        <v>4573</v>
       </c>
     </row>
     <row r="333" ht="11" customHeight="true" outlineLevel="3">
       <c r="B333" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="C333" s="11" t="n">
-        <v>21</v>
+      <c r="C333" s="16" t="n">
+        <v>1756</v>
       </c>
     </row>
     <row r="334" ht="11" customHeight="true" outlineLevel="3">
@@ -4148,15 +4154,15 @@
         <v>333</v>
       </c>
       <c r="C334" s="11" t="n">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="335" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B335" s="15" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="335" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B335" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="C335" s="11" t="n">
-        <v>7</v>
+      <c r="C335" s="12" t="n">
+        <v>2155</v>
       </c>
     </row>
     <row r="336" ht="11" customHeight="true" outlineLevel="3">
@@ -4164,23 +4170,23 @@
         <v>335</v>
       </c>
       <c r="C336" s="11" t="n">
-        <v>445</v>
+        <v>21</v>
       </c>
     </row>
     <row r="337" ht="11" customHeight="true" outlineLevel="3">
       <c r="B337" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="C337" s="16" t="n">
-        <v>1634</v>
-      </c>
-    </row>
-    <row r="338" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B338" s="14" t="s">
+      <c r="C337" s="11" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="338" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B338" s="15" t="s">
         <v>337</v>
       </c>
-      <c r="C338" s="12" t="n">
-        <v>122171</v>
+      <c r="C338" s="11" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="339" ht="11" customHeight="true" outlineLevel="3">
@@ -4188,31 +4194,31 @@
         <v>338</v>
       </c>
       <c r="C339" s="11" t="n">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="340" ht="22" customHeight="true" outlineLevel="3">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="340" ht="11" customHeight="true" outlineLevel="3">
       <c r="B340" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="C340" s="11" t="n">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="341" ht="22" customHeight="true" outlineLevel="3">
-      <c r="B341" s="15" t="s">
+      <c r="C340" s="16" t="n">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="341" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B341" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="C341" s="11" t="n">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="342" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C341" s="12" t="n">
+        <v>115641</v>
+      </c>
+    </row>
+    <row r="342" ht="11" customHeight="true" outlineLevel="3">
       <c r="B342" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="C342" s="16" t="n">
-        <v>3833</v>
+      <c r="C342" s="11" t="n">
+        <v>292</v>
       </c>
     </row>
     <row r="343" ht="22" customHeight="true" outlineLevel="3">
@@ -4220,7 +4226,7 @@
         <v>342</v>
       </c>
       <c r="C343" s="11" t="n">
-        <v>180</v>
+        <v>602</v>
       </c>
     </row>
     <row r="344" ht="22" customHeight="true" outlineLevel="3">
@@ -4228,7 +4234,7 @@
         <v>343</v>
       </c>
       <c r="C344" s="11" t="n">
-        <v>120</v>
+        <v>48</v>
       </c>
     </row>
     <row r="345" ht="22" customHeight="true" outlineLevel="3">
@@ -4236,7 +4242,7 @@
         <v>344</v>
       </c>
       <c r="C345" s="16" t="n">
-        <v>3971</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="346" ht="22" customHeight="true" outlineLevel="3">
@@ -4244,7 +4250,7 @@
         <v>345</v>
       </c>
       <c r="C346" s="11" t="n">
-        <v>205</v>
+        <v>580</v>
       </c>
     </row>
     <row r="347" ht="22" customHeight="true" outlineLevel="3">
@@ -4252,31 +4258,31 @@
         <v>346</v>
       </c>
       <c r="C347" s="11" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="348" ht="11" customHeight="true" outlineLevel="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="348" ht="22" customHeight="true" outlineLevel="3">
       <c r="B348" s="15" t="s">
         <v>347</v>
       </c>
-      <c r="C348" s="11" t="n">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="349" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C348" s="16" t="n">
+        <v>3785</v>
+      </c>
+    </row>
+    <row r="349" ht="22" customHeight="true" outlineLevel="3">
       <c r="B349" s="15" t="s">
         <v>348</v>
       </c>
-      <c r="C349" s="16" t="n">
-        <v>1444</v>
-      </c>
-    </row>
-    <row r="350" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C349" s="11" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="350" ht="22" customHeight="true" outlineLevel="3">
       <c r="B350" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="C350" s="16" t="n">
-        <v>2326</v>
+      <c r="C350" s="11" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="351" ht="11" customHeight="true" outlineLevel="3">
@@ -4284,31 +4290,31 @@
         <v>350</v>
       </c>
       <c r="C351" s="11" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="352" ht="22" customHeight="true" outlineLevel="3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="352" ht="11" customHeight="true" outlineLevel="3">
       <c r="B352" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="C352" s="11" t="n">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="353" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C352" s="16" t="n">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="353" ht="11" customHeight="true" outlineLevel="3">
       <c r="B353" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="C353" s="11" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="354" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C353" s="16" t="n">
+        <v>2198</v>
+      </c>
+    </row>
+    <row r="354" ht="11" customHeight="true" outlineLevel="3">
       <c r="B354" s="15" t="s">
         <v>353</v>
       </c>
       <c r="C354" s="11" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="355" ht="22" customHeight="true" outlineLevel="3">
@@ -4316,7 +4322,7 @@
         <v>354</v>
       </c>
       <c r="C355" s="11" t="n">
-        <v>476</v>
+        <v>738</v>
       </c>
     </row>
     <row r="356" ht="22" customHeight="true" outlineLevel="3">
@@ -4324,15 +4330,15 @@
         <v>355</v>
       </c>
       <c r="C356" s="11" t="n">
-        <v>120</v>
+        <v>476</v>
       </c>
     </row>
     <row r="357" ht="22" customHeight="true" outlineLevel="3">
       <c r="B357" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C357" s="16" t="n">
-        <v>4609</v>
+      <c r="C357" s="11" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="358" ht="22" customHeight="true" outlineLevel="3">
@@ -4340,7 +4346,7 @@
         <v>357</v>
       </c>
       <c r="C358" s="11" t="n">
-        <v>484</v>
+        <v>435</v>
       </c>
     </row>
     <row r="359" ht="22" customHeight="true" outlineLevel="3">
@@ -4348,15 +4354,15 @@
         <v>358</v>
       </c>
       <c r="C359" s="11" t="n">
-        <v>416</v>
+        <v>120</v>
       </c>
     </row>
     <row r="360" ht="22" customHeight="true" outlineLevel="3">
       <c r="B360" s="15" t="s">
         <v>359</v>
       </c>
-      <c r="C360" s="11" t="n">
-        <v>48</v>
+      <c r="C360" s="16" t="n">
+        <v>4393</v>
       </c>
     </row>
     <row r="361" ht="22" customHeight="true" outlineLevel="3">
@@ -4364,7 +4370,7 @@
         <v>360</v>
       </c>
       <c r="C361" s="11" t="n">
-        <v>448</v>
+        <v>415</v>
       </c>
     </row>
     <row r="362" ht="22" customHeight="true" outlineLevel="3">
@@ -4372,7 +4378,7 @@
         <v>361</v>
       </c>
       <c r="C362" s="11" t="n">
-        <v>726</v>
+        <v>5</v>
       </c>
     </row>
     <row r="363" ht="22" customHeight="true" outlineLevel="3">
@@ -4380,7 +4386,7 @@
         <v>362</v>
       </c>
       <c r="C363" s="11" t="n">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="364" ht="22" customHeight="true" outlineLevel="3">
@@ -4388,15 +4394,15 @@
         <v>363</v>
       </c>
       <c r="C364" s="11" t="n">
-        <v>48</v>
+        <v>448</v>
       </c>
     </row>
     <row r="365" ht="22" customHeight="true" outlineLevel="3">
       <c r="B365" s="15" t="s">
         <v>364</v>
       </c>
-      <c r="C365" s="16" t="n">
-        <v>10113</v>
+      <c r="C365" s="11" t="n">
+        <v>561</v>
       </c>
     </row>
     <row r="366" ht="22" customHeight="true" outlineLevel="3">
@@ -4404,63 +4410,63 @@
         <v>365</v>
       </c>
       <c r="C366" s="11" t="n">
-        <v>22</v>
+        <v>179</v>
       </c>
     </row>
     <row r="367" ht="22" customHeight="true" outlineLevel="3">
       <c r="B367" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="C367" s="16" t="n">
-        <v>1517</v>
+      <c r="C367" s="11" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="368" ht="22" customHeight="true" outlineLevel="3">
       <c r="B368" s="15" t="s">
         <v>367</v>
       </c>
-      <c r="C368" s="11" t="n">
-        <v>48</v>
+      <c r="C368" s="16" t="n">
+        <v>9947</v>
       </c>
     </row>
     <row r="369" ht="22" customHeight="true" outlineLevel="3">
       <c r="B369" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="C369" s="16" t="n">
-        <v>4630</v>
+      <c r="C369" s="11" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="370" ht="22" customHeight="true" outlineLevel="3">
       <c r="B370" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="C370" s="11" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="371" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C370" s="16" t="n">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="371" ht="22" customHeight="true" outlineLevel="3">
       <c r="B371" s="15" t="s">
         <v>370</v>
       </c>
       <c r="C371" s="11" t="n">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="372" ht="11" customHeight="true" outlineLevel="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="372" ht="22" customHeight="true" outlineLevel="3">
       <c r="B372" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="C372" s="11" t="n">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="373" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C372" s="16" t="n">
+        <v>4259</v>
+      </c>
+    </row>
+    <row r="373" ht="22" customHeight="true" outlineLevel="3">
       <c r="B373" s="15" t="s">
         <v>372</v>
       </c>
       <c r="C373" s="11" t="n">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="374" ht="11" customHeight="true" outlineLevel="3">
@@ -4468,7 +4474,7 @@
         <v>373</v>
       </c>
       <c r="C374" s="11" t="n">
-        <v>2</v>
+        <v>787</v>
       </c>
     </row>
     <row r="375" ht="11" customHeight="true" outlineLevel="3">
@@ -4476,31 +4482,31 @@
         <v>374</v>
       </c>
       <c r="C375" s="11" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="376" ht="22" customHeight="true" outlineLevel="3">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="376" ht="11" customHeight="true" outlineLevel="3">
       <c r="B376" s="15" t="s">
         <v>375</v>
       </c>
       <c r="C376" s="11" t="n">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="377" ht="22" customHeight="true" outlineLevel="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="377" ht="11" customHeight="true" outlineLevel="3">
       <c r="B377" s="15" t="s">
         <v>376</v>
       </c>
       <c r="C377" s="11" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="378" ht="22" customHeight="true" outlineLevel="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="378" ht="11" customHeight="true" outlineLevel="3">
       <c r="B378" s="15" t="s">
         <v>377</v>
       </c>
       <c r="C378" s="11" t="n">
-        <v>220</v>
+        <v>990</v>
       </c>
     </row>
     <row r="379" ht="22" customHeight="true" outlineLevel="3">
@@ -4508,15 +4514,15 @@
         <v>378</v>
       </c>
       <c r="C379" s="11" t="n">
-        <v>24</v>
+        <v>195</v>
       </c>
     </row>
     <row r="380" ht="22" customHeight="true" outlineLevel="3">
       <c r="B380" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="C380" s="16" t="n">
-        <v>3102</v>
+      <c r="C380" s="11" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="381" ht="22" customHeight="true" outlineLevel="3">
@@ -4524,39 +4530,39 @@
         <v>380</v>
       </c>
       <c r="C381" s="11" t="n">
-        <v>48</v>
+        <v>216</v>
       </c>
     </row>
     <row r="382" ht="22" customHeight="true" outlineLevel="3">
       <c r="B382" s="15" t="s">
         <v>381</v>
       </c>
-      <c r="C382" s="16" t="n">
-        <v>2606</v>
-      </c>
-    </row>
-    <row r="383" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C382" s="11" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="383" ht="22" customHeight="true" outlineLevel="3">
       <c r="B383" s="15" t="s">
         <v>382</v>
       </c>
-      <c r="C383" s="11" t="n">
-        <v>256</v>
+      <c r="C383" s="16" t="n">
+        <v>3153</v>
       </c>
     </row>
     <row r="384" ht="22" customHeight="true" outlineLevel="3">
       <c r="B384" s="15" t="s">
         <v>383</v>
       </c>
-      <c r="C384" s="16" t="n">
-        <v>5282</v>
-      </c>
-    </row>
-    <row r="385" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C384" s="11" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="385" ht="22" customHeight="true" outlineLevel="3">
       <c r="B385" s="15" t="s">
         <v>384</v>
       </c>
-      <c r="C385" s="11" t="n">
-        <v>561</v>
+      <c r="C385" s="16" t="n">
+        <v>2536</v>
       </c>
     </row>
     <row r="386" ht="11" customHeight="true" outlineLevel="3">
@@ -4564,7 +4570,7 @@
         <v>385</v>
       </c>
       <c r="C386" s="11" t="n">
-        <v>40</v>
+        <v>256</v>
       </c>
     </row>
     <row r="387" ht="22" customHeight="true" outlineLevel="3">
@@ -4572,7 +4578,7 @@
         <v>386</v>
       </c>
       <c r="C387" s="11" t="n">
-        <v>169</v>
+        <v>622</v>
       </c>
     </row>
     <row r="388" ht="11" customHeight="true" outlineLevel="3">
@@ -4580,15 +4586,15 @@
         <v>387</v>
       </c>
       <c r="C388" s="11" t="n">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="389" ht="22" customHeight="true" outlineLevel="3">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="389" ht="11" customHeight="true" outlineLevel="3">
       <c r="B389" s="15" t="s">
         <v>388</v>
       </c>
       <c r="C389" s="11" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="390" ht="22" customHeight="true" outlineLevel="3">
@@ -4596,7 +4602,7 @@
         <v>389</v>
       </c>
       <c r="C390" s="11" t="n">
-        <v>919</v>
+        <v>98</v>
       </c>
     </row>
     <row r="391" ht="11" customHeight="true" outlineLevel="3">
@@ -4604,7 +4610,7 @@
         <v>390</v>
       </c>
       <c r="C391" s="11" t="n">
-        <v>546</v>
+        <v>898</v>
       </c>
     </row>
     <row r="392" ht="22" customHeight="true" outlineLevel="3">
@@ -4612,31 +4618,31 @@
         <v>391</v>
       </c>
       <c r="C392" s="11" t="n">
-        <v>200</v>
+        <v>669</v>
       </c>
     </row>
     <row r="393" ht="11" customHeight="true" outlineLevel="3">
       <c r="B393" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C393" s="16" t="n">
-        <v>3373</v>
-      </c>
-    </row>
-    <row r="394" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C393" s="11" t="n">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="394" ht="22" customHeight="true" outlineLevel="3">
       <c r="B394" s="15" t="s">
         <v>393</v>
       </c>
-      <c r="C394" s="16" t="n">
-        <v>1783</v>
+      <c r="C394" s="11" t="n">
+        <v>167</v>
       </c>
     </row>
     <row r="395" ht="11" customHeight="true" outlineLevel="3">
       <c r="B395" s="15" t="s">
         <v>394</v>
       </c>
-      <c r="C395" s="11" t="n">
-        <v>12</v>
+      <c r="C395" s="16" t="n">
+        <v>3058</v>
       </c>
     </row>
     <row r="396" ht="11" customHeight="true" outlineLevel="3">
@@ -4644,7 +4650,7 @@
         <v>395</v>
       </c>
       <c r="C396" s="16" t="n">
-        <v>1680</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="397" ht="11" customHeight="true" outlineLevel="3">
@@ -4652,31 +4658,31 @@
         <v>396</v>
       </c>
       <c r="C397" s="11" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="398" ht="22" customHeight="true" outlineLevel="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="398" ht="11" customHeight="true" outlineLevel="3">
       <c r="B398" s="15" t="s">
         <v>397</v>
       </c>
       <c r="C398" s="16" t="n">
-        <v>2571</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="399" ht="11" customHeight="true" outlineLevel="3">
       <c r="B399" s="15" t="s">
         <v>398</v>
       </c>
-      <c r="C399" s="16" t="n">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="400" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C399" s="11" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="400" ht="22" customHeight="true" outlineLevel="3">
       <c r="B400" s="15" t="s">
         <v>399</v>
       </c>
       <c r="C400" s="16" t="n">
-        <v>4100</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="401" ht="11" customHeight="true" outlineLevel="3">
@@ -4684,23 +4690,23 @@
         <v>400</v>
       </c>
       <c r="C401" s="16" t="n">
-        <v>4365</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="402" ht="11" customHeight="true" outlineLevel="3">
       <c r="B402" s="15" t="s">
         <v>401</v>
       </c>
-      <c r="C402" s="11" t="n">
-        <v>50</v>
+      <c r="C402" s="16" t="n">
+        <v>3762</v>
       </c>
     </row>
     <row r="403" ht="11" customHeight="true" outlineLevel="3">
       <c r="B403" s="15" t="s">
         <v>402</v>
       </c>
-      <c r="C403" s="11" t="n">
-        <v>369</v>
+      <c r="C403" s="16" t="n">
+        <v>4358</v>
       </c>
     </row>
     <row r="404" ht="11" customHeight="true" outlineLevel="3">
@@ -4716,7 +4722,7 @@
         <v>404</v>
       </c>
       <c r="C405" s="11" t="n">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="406" ht="11" customHeight="true" outlineLevel="3">
@@ -4724,23 +4730,23 @@
         <v>405</v>
       </c>
       <c r="C406" s="11" t="n">
-        <v>511</v>
+        <v>50</v>
       </c>
     </row>
     <row r="407" ht="11" customHeight="true" outlineLevel="3">
       <c r="B407" s="15" t="s">
         <v>406</v>
       </c>
-      <c r="C407" s="16" t="n">
-        <v>4160</v>
-      </c>
-    </row>
-    <row r="408" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C407" s="11" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="408" ht="11" customHeight="true" outlineLevel="3">
       <c r="B408" s="15" t="s">
         <v>407</v>
       </c>
-      <c r="C408" s="16" t="n">
-        <v>12692</v>
+      <c r="C408" s="11" t="n">
+        <v>353</v>
       </c>
     </row>
     <row r="409" ht="11" customHeight="true" outlineLevel="3">
@@ -4748,31 +4754,47 @@
         <v>408</v>
       </c>
       <c r="C409" s="16" t="n">
-        <v>11761</v>
+        <v>4067</v>
       </c>
     </row>
     <row r="410" ht="22" customHeight="true" outlineLevel="3">
       <c r="B410" s="15" t="s">
         <v>409</v>
       </c>
-      <c r="C410" s="11" t="n">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="411" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C410" s="16" t="n">
+        <v>12076</v>
+      </c>
+    </row>
+    <row r="411" ht="11" customHeight="true" outlineLevel="3">
       <c r="B411" s="15" t="s">
         <v>410</v>
       </c>
-      <c r="C411" s="11" t="n">
-        <v>156</v>
+      <c r="C411" s="16" t="n">
+        <v>11758</v>
       </c>
     </row>
     <row r="412" ht="22" customHeight="true" outlineLevel="3">
       <c r="B412" s="15" t="s">
         <v>411</v>
       </c>
-      <c r="C412" s="16" t="n">
-        <v>18036</v>
+      <c r="C412" s="11" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="413" ht="22" customHeight="true" outlineLevel="3">
+      <c r="B413" s="15" t="s">
+        <v>412</v>
+      </c>
+      <c r="C413" s="11" t="n">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="414" ht="22" customHeight="true" outlineLevel="3">
+      <c r="B414" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="C414" s="16" t="n">
+        <v>17724</v>
       </c>
     </row>
   </sheetData>

</xml_diff>